<commit_message>
xlsx personal data removed
</commit_message>
<xml_diff>
--- a/data/Vorkurs_22_with_brocanto_transposed.xlsx
+++ b/data/Vorkurs_22_with_brocanto_transposed.xlsx
@@ -2,15 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Documents\Forschung\Broca-Paper\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04BD2FB-C2FE-486B-97EF-65816D5FE3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82675012-3EF6-4639-8D9A-44A1814D366D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,9 +433,9 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>1</v>
       </c>
@@ -487,7 +482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -537,7 +532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -587,7 +582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -637,7 +632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -687,7 +682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -737,7 +732,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -787,7 +782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -837,7 +832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -887,7 +882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -937,7 +932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -987,7 +982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1037,10 +1032,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
     </row>
   </sheetData>

</xml_diff>